<commit_message>
Alias monte.mean and monte.average. Screen updating failed attempts. Move FSM logic to monte.h
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -33,6 +33,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="mm\.ss.0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -68,8 +71,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,27 +627,112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32FF5F26-4349-477D-8AA4-58B7159FDB22}">
-  <dimension ref="B2:E5"/>
+  <dimension ref="B2:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="5" max="5" width="10.59765625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.45">
       <c r="D2">
         <f ca="1">RAND()</f>
-        <v>0.60178134372956893</v>
+        <v>0.43294917162275903</v>
       </c>
       <c r="E2">
         <f ca="1">_xll.MONTE.MEAN(D2)</f>
-        <v>0.49780885601414315</v>
+        <v>0.49858219648350982</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="E3">
+        <f t="array" aca="1" ref="E3:F3" ca="1">_xll.MONTE.MEAN(D2)</f>
+        <v>0.49858219648350982</v>
+      </c>
+      <c r="F3">
+        <f ca="1"/>
+        <v>16506</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="E4">
+        <f ca="1">(E6*F6+E7*F7)/(F6+F7)</f>
+        <v>0.49858219648351021</v>
+      </c>
+      <c r="F4">
+        <f ca="1">SUM(F6:F7)</f>
+        <v>16506</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>0</v>
+      </c>
+      <c r="E5">
+        <f ca="1">E3-E4</f>
+        <v>0</v>
+      </c>
+      <c r="F5" t="b">
+        <f ca="1">F3=F4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="E6">
+        <f t="array" aca="1" ref="E6:F6" ca="1">_xll.MONTE.WHEN(D2&gt;0.5, _xll.MONTE.MEAN(D2))</f>
+        <v>0.74947916156012151</v>
+      </c>
+      <c r="F6">
+        <f ca="1"/>
+        <v>8210</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B7">
+        <f ca="1">_xll.MONTE.COUNT()</f>
+        <v>16506</v>
+      </c>
+      <c r="E7">
+        <f t="array" aca="1" ref="E7:F7" ca="1">_xll.MONTE.WHEN(D2&lt;0.5, _xll.MONTE.MEAN(D2))</f>
+        <v>0.25028614015769313</v>
+      </c>
+      <c r="F7">
+        <f ca="1"/>
+        <v>8296</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="B8" s="1">
+        <f ca="1">_xll.MONTE.ELAPSED()/86400</f>
+        <v>6.0763908550143242E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="E9">
+        <f t="array" aca="1" ref="E9:F9" ca="1">_xll.MONTE.STDEV(D2)</f>
+        <v>0.49858219648350982</v>
+      </c>
+      <c r="F9">
+        <f ca="1"/>
+        <v>0.28828992120682762</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.45">
+      <c r="E10">
+        <f t="array" aca="1" ref="E10:G10" ca="1">_xll.MONTE.STDEV(D2)</f>
+        <v>0.49858219648350982</v>
+      </c>
+      <c r="F10">
+        <f ca="1"/>
+        <v>0.28828992120682762</v>
+      </c>
+      <c r="G10">
+        <f ca="1"/>
+        <v>16506</v>
       </c>
     </row>
   </sheetData>

</xml_diff>